<commit_message>
add unit db for managing status, untested
</commit_message>
<xml_diff>
--- a/project_tracker.xlsx
+++ b/project_tracker.xlsx
@@ -181,7 +181,7 @@
     <t xml:space="preserve">Can take many pictures of parrot anafi as test</t>
   </si>
   <si>
-    <t xml:space="preserve">Train model on dataset</t>
+    <t xml:space="preserve">Create &amp; train model on dataset</t>
   </si>
   <si>
     <t xml:space="preserve">Image recognition test</t>
@@ -512,8 +512,8 @@
   </sheetPr>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
some UI changes and embedded video stream to unit detail page
</commit_message>
<xml_diff>
--- a/project_tracker.xlsx
+++ b/project_tracker.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
   <si>
     <t xml:space="preserve">TASK TRACKER</t>
   </si>
@@ -232,14 +232,15 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
-    <numFmt numFmtId="165" formatCode="dd\-mmm"/>
-    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="dd\-mmm"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -258,15 +259,17 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="10"/>
+      <color rgb="FF17176B"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -275,18 +278,7 @@
       <color rgb="FF2117DE"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF17176B"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -305,6 +297,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF000042"/>
+        <bgColor rgb="FF000080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0C78C"/>
+        <bgColor rgb="FFFFB66C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFD1"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF158466"/>
         <bgColor rgb="FF008080"/>
       </patternFill>
@@ -319,24 +329,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFD1"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000042"/>
-        <bgColor rgb="FF000080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF0C78C"/>
-        <bgColor rgb="FFFFB66C"/>
       </patternFill>
     </fill>
     <fill>
@@ -367,45 +359,23 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="hair">
-        <color rgb="FF000080"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF000080"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF000080"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="hair">
         <color rgb="FF000080"/>
       </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="hair">
         <color rgb="FF000080"/>
       </left>
       <right/>
-      <top style="hair">
-        <color rgb="FF000080"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="hair">
-        <color rgb="FF000080"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="hair">
+        <color rgb="FF000080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -413,10 +383,10 @@
       <right style="hair">
         <color rgb="FF000080"/>
       </right>
-      <top style="hair">
-        <color rgb="FF000080"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="hair">
+        <color rgb="FF000080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -440,10 +410,10 @@
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
-      <top/>
-      <bottom style="hair">
-        <color rgb="FF000080"/>
-      </bottom>
+      <top style="hair">
+        <color rgb="FF000080"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -451,10 +421,10 @@
         <color rgb="FF000080"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="hair">
-        <color rgb="FF000080"/>
-      </bottom>
+      <top style="hair">
+        <color rgb="FF000080"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -462,10 +432,32 @@
       <right style="hair">
         <color rgb="FF000080"/>
       </right>
-      <top/>
+      <top style="hair">
+        <color rgb="FF000080"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF000080"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000080"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000080"/>
+      </top>
       <bottom style="hair">
         <color rgb="FF000080"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -494,59 +486,59 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="9" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="5" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="10" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="9" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="10">
@@ -558,35 +550,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -598,24 +590,24 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Untitled1" xfId="20"/>
-    <cellStyle name="Untitled2" xfId="21"/>
-    <cellStyle name="Untitled3" xfId="22"/>
-    <cellStyle name="Untitled4" xfId="23"/>
-    <cellStyle name="Result2" xfId="24"/>
-    <cellStyle name="Heading1" xfId="25"/>
-    <cellStyle name="Background" xfId="26"/>
-    <cellStyle name="Card" xfId="27"/>
-    <cellStyle name="Input" xfId="28"/>
-    <cellStyle name="Card TL" xfId="29"/>
-    <cellStyle name="Card T" xfId="30"/>
-    <cellStyle name="Card TR" xfId="31"/>
-    <cellStyle name="Card L" xfId="32"/>
-    <cellStyle name="Card R" xfId="33"/>
-    <cellStyle name="Card B" xfId="34"/>
-    <cellStyle name="Card BL" xfId="35"/>
-    <cellStyle name="Card BR" xfId="36"/>
-    <cellStyle name="Column Header" xfId="37"/>
+    <cellStyle name="Background" xfId="20"/>
+    <cellStyle name="Card" xfId="21"/>
+    <cellStyle name="Card B" xfId="22"/>
+    <cellStyle name="Card BL" xfId="23"/>
+    <cellStyle name="Card BR" xfId="24"/>
+    <cellStyle name="Card L" xfId="25"/>
+    <cellStyle name="Card R" xfId="26"/>
+    <cellStyle name="Card T" xfId="27"/>
+    <cellStyle name="Card TL" xfId="28"/>
+    <cellStyle name="Card TR" xfId="29"/>
+    <cellStyle name="Column Header" xfId="30"/>
+    <cellStyle name="Heading1" xfId="31"/>
+    <cellStyle name="Input" xfId="32"/>
+    <cellStyle name="Result2" xfId="33"/>
+    <cellStyle name="Untitled1" xfId="34"/>
+    <cellStyle name="Untitled2" xfId="35"/>
+    <cellStyle name="Untitled3" xfId="36"/>
+    <cellStyle name="Untitled4" xfId="37"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -716,7 +708,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -845,7 +837,9 @@
       <c r="G6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="I6" s="5" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
data management files added to dir
</commit_message>
<xml_diff>
--- a/project_tracker.xlsx
+++ b/project_tracker.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
   <si>
     <t xml:space="preserve">TASK TRACKER</t>
   </si>
@@ -61,18 +61,18 @@
     <t xml:space="preserve">Backend communication framework between hub + units</t>
   </si>
   <si>
+    <t xml:space="preserve">See readme for explanation of function/directories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connect &amp; test servos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flash ardurover</t>
+  </si>
+  <si>
     <t xml:space="preserve">IN PROGRESS</t>
   </si>
   <si>
-    <t xml:space="preserve">See readme for explanation of function/directories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connect &amp; test servos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flash ardurover</t>
-  </si>
-  <si>
     <t xml:space="preserve">Current board still has INAV</t>
   </si>
   <si>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Assemble RC components and connect together</t>
   </si>
   <si>
-    <t xml:space="preserve">Using PQ-2</t>
+    <t xml:space="preserve">Using PQ-2 model (once built)</t>
   </si>
   <si>
     <t xml:space="preserve">Telegram bot</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">Test power pi from 5V pin on FC</t>
   </si>
   <si>
-    <t xml:space="preserve">Make sure to test SDR function. Can also use 18650 in battery shield</t>
+    <t xml:space="preserve">Perhaps better to use 18650 with shield? Compare FC pin with this</t>
   </si>
   <si>
     <t xml:space="preserve">Test issue commands to unit from dislocated network</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">Telemetry over 4G</t>
   </si>
   <si>
-    <t xml:space="preserve">Ardupilot telemetry over 4G</t>
+    <t xml:space="preserve">Seems to work fine over VPN</t>
   </si>
   <si>
     <t xml:space="preserve">Autorotation</t>
@@ -244,7 +244,7 @@
     <t xml:space="preserve">Design servo mount and pi/camera case</t>
   </si>
   <si>
-    <t xml:space="preserve">Current idea: servo in mount below with splayed floorstands; pi, SDR, cam etc in case on top</t>
+    <t xml:space="preserve">Have designed a payload container for testing for now, later need to design with servo mounts &amp; rotating camera</t>
   </si>
   <si>
     <t xml:space="preserve">CREATE MASTER SD CARD</t>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t xml:space="preserve">Print</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Printing provisional/testing Rpi payload container</t>
   </si>
   <si>
     <t xml:space="preserve">Assemble</t>
@@ -747,7 +750,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -856,25 +859,25 @@
         <v>12</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>17</v>
@@ -883,7 +886,7 @@
         <v>18</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>19</v>
@@ -903,7 +906,7 @@
         <v>22</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>23</v>
@@ -912,7 +915,7 @@
         <v>24</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>25</v>
@@ -923,7 +926,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>27</v>
@@ -950,7 +953,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>33</v>
@@ -966,7 +969,7 @@
         <v>36</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>37</v>
@@ -986,7 +989,7 @@
         <v>40</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>41</v>
@@ -1006,7 +1009,9 @@
       <c r="D11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="F11" s="6" t="s">
         <v>45</v>
       </c>
@@ -1026,7 +1031,7 @@
         <v>48</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>49</v>
@@ -1128,7 +1133,7 @@
         <v>60</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>61</v>
@@ -1161,7 +1166,9 @@
       <c r="A21" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="8"/>
+      <c r="B21" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="C21" s="8" t="s">
         <v>65</v>
       </c>
@@ -1172,18 +1179,22 @@
         <v>66</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="B22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -1191,9 +1202,9 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1206,7 +1217,7 @@
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>

</xml_diff>